<commit_message>
Multiple correction in documentation.
</commit_message>
<xml_diff>
--- a/Documentation/geschwindigkeitsberechnung.xlsx
+++ b/Documentation/geschwindigkeitsberechnung.xlsx
@@ -1,40 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20910"/>
+  <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="15120" windowHeight="8010"/>
+    <workbookView xWindow="3960" yWindow="1800" windowWidth="23420" windowHeight="14920"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t>Distanz</t>
-  </si>
-  <si>
-    <t>Zeitmessung 1</t>
-  </si>
-  <si>
-    <t>Zeitmessung 2</t>
-  </si>
-  <si>
-    <t>Zeitmessung 3</t>
-  </si>
-  <si>
-    <t>Zeitmessung 4</t>
-  </si>
-  <si>
-    <t>Zeitmessung 5</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Durchschnitt</t>
   </si>
@@ -47,12 +34,18 @@
   <si>
     <t>Skalierung</t>
   </si>
+  <si>
+    <t>Distanz (m)</t>
+  </si>
+  <si>
+    <t>Zeitmessung (s)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -60,16 +53,51 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -77,14 +105,64 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="11">
+    <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -376,151 +454,193 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="13.33203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="31.140625" customWidth="1"/>
-    <col min="3" max="7" width="14.42578125" customWidth="1"/>
-    <col min="8" max="8" width="14" customWidth="1"/>
-    <col min="9" max="9" width="28.5703125" customWidth="1"/>
+    <col min="1" max="1" width="3" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" style="1"/>
+    <col min="3" max="3" width="17.1640625" style="1" customWidth="1"/>
+    <col min="4" max="8" width="8.5" style="1" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" style="1"/>
+    <col min="10" max="11" width="14.83203125" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="13.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" t="s">
+    <row r="2" spans="2:11" ht="35" customHeight="1">
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" ht="35" customHeight="1">
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="3">
+        <v>1</v>
+      </c>
+      <c r="E3" s="3">
+        <v>2</v>
+      </c>
+      <c r="F3" s="3">
+        <v>3</v>
+      </c>
+      <c r="G3" s="3">
+        <v>4</v>
+      </c>
+      <c r="H3" s="3">
+        <v>5</v>
+      </c>
+      <c r="I3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
     </row>
-    <row r="2" spans="1:10">
-      <c r="A2">
+    <row r="4" spans="2:11" ht="35" customHeight="1">
+      <c r="B4" s="4">
         <v>500</v>
       </c>
-      <c r="B2">
+      <c r="C4" s="4">
         <v>100</v>
       </c>
-      <c r="C2">
+      <c r="D4" s="4">
         <v>24.7</v>
       </c>
-      <c r="D2">
+      <c r="E4" s="4">
         <v>25</v>
       </c>
-      <c r="E2">
+      <c r="F4" s="4">
         <v>24.9</v>
       </c>
-      <c r="F2">
+      <c r="G4" s="4">
         <v>25</v>
       </c>
-      <c r="G2">
+      <c r="H4" s="4">
         <v>24.9</v>
       </c>
-      <c r="H2">
-        <f>AVERAGE(C2:G2)</f>
+      <c r="I4" s="4">
+        <f>AVERAGE(D4:H4)</f>
         <v>24.9</v>
       </c>
-      <c r="I2">
-        <f>A2/H2*3.6</f>
+      <c r="J4" s="4">
+        <f>B4/I4*3.6</f>
         <v>72.289156626506028</v>
       </c>
-      <c r="J2">
-        <f>I2/B2</f>
+      <c r="K4" s="5">
+        <f>J4/C4</f>
         <v>0.72289156626506024</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
-      <c r="A3">
+    <row r="5" spans="2:11" ht="35" customHeight="1">
+      <c r="B5" s="4">
         <v>500</v>
       </c>
-      <c r="B3">
+      <c r="C5" s="4">
         <v>175</v>
       </c>
-      <c r="C3">
+      <c r="D5" s="4">
         <v>14.2</v>
       </c>
-      <c r="D3">
+      <c r="E5" s="4">
         <v>14.2</v>
       </c>
-      <c r="E3">
+      <c r="F5" s="4">
         <v>14.2</v>
       </c>
-      <c r="F3">
+      <c r="G5" s="4">
         <v>14.2</v>
       </c>
-      <c r="G3">
+      <c r="H5" s="4">
         <v>14.2</v>
       </c>
-      <c r="H3">
-        <f>AVERAGE(C3:G3)</f>
+      <c r="I5" s="4">
+        <f>AVERAGE(D5:H5)</f>
         <v>14.2</v>
       </c>
-      <c r="I3">
-        <f>A3/H3*3.6</f>
+      <c r="J5" s="4">
+        <f>B5/I5*3.6</f>
         <v>126.76056338028171</v>
       </c>
-      <c r="J3">
-        <f>I3/B3</f>
+      <c r="K5" s="5">
+        <f>J5/C5</f>
         <v>0.7243460764587526</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="D2:I2"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="K2:K3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <ignoredErrors>
+    <ignoredError sqref="I4:I5" formulaRange="1"/>
+  </ignoredErrors>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>